<commit_message>
updated statistics using new TRREB data
</commit_message>
<xml_diff>
--- a/Exploratory Analysis/Statistics/CondoListings_Statistics_2018to2019.xlsx
+++ b/Exploratory Analysis/Statistics/CondoListings_Statistics_2018to2019.xlsx
@@ -491,28 +491,28 @@
         <v>14</v>
       </c>
       <c r="C2">
-        <v>405436.4240980259</v>
+        <v>423182.0660165041</v>
       </c>
       <c r="D2">
-        <v>405201.6414363512</v>
+        <v>423639.1464891222</v>
       </c>
       <c r="E2">
-        <v>774.9911202185792</v>
+        <v>763.6294073518379</v>
       </c>
       <c r="F2">
-        <v>419900</v>
+        <v>429000</v>
       </c>
       <c r="G2">
-        <v>423000</v>
+        <v>430000</v>
       </c>
       <c r="H2">
-        <v>749</v>
+        <v>649</v>
       </c>
       <c r="I2">
-        <v>1469</v>
+        <v>1333</v>
       </c>
       <c r="J2">
-        <v>522.85</v>
+        <v>554.77</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -521,28 +521,28 @@
         <v>15</v>
       </c>
       <c r="C3">
-        <v>410880.3002444988</v>
+        <v>427502.9215053763</v>
       </c>
       <c r="D3">
-        <v>407092.0021026895</v>
+        <v>424099.6974731183</v>
       </c>
       <c r="E3">
-        <v>774.2453385672228</v>
+        <v>762.8306451612904</v>
       </c>
       <c r="F3">
-        <v>425000</v>
+        <v>429900</v>
       </c>
       <c r="G3">
-        <v>423250</v>
+        <v>430000</v>
       </c>
       <c r="H3">
-        <v>749</v>
+        <v>649</v>
       </c>
       <c r="I3">
-        <v>2045</v>
+        <v>1860</v>
       </c>
       <c r="J3">
-        <v>525.79</v>
+        <v>555.96</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -551,28 +551,28 @@
         <v>16</v>
       </c>
       <c r="C4">
-        <v>409990.467251462</v>
+        <v>426933.6651612903</v>
       </c>
       <c r="D4">
-        <v>405104.449</v>
+        <v>422437.3082516129</v>
       </c>
       <c r="E4">
-        <v>797.2117302052786</v>
+        <v>789.2909677419354</v>
       </c>
       <c r="F4">
-        <v>424900</v>
+        <v>429900</v>
       </c>
       <c r="G4">
-        <v>420000</v>
+        <v>429000</v>
       </c>
       <c r="H4">
         <v>749</v>
       </c>
       <c r="I4">
-        <v>1710</v>
+        <v>1550</v>
       </c>
       <c r="J4">
-        <v>508.15</v>
+        <v>535.21</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -910,28 +910,28 @@
         <v>17</v>
       </c>
       <c r="C2">
-        <v>411575.7532029669</v>
+        <v>428194.3145817913</v>
       </c>
       <c r="D2">
-        <v>408616.4861766689</v>
+        <v>425550.5336787565</v>
       </c>
       <c r="E2">
-        <v>799.7807196198235</v>
+        <v>792.4122871946706</v>
       </c>
       <c r="F2">
-        <v>428888</v>
+        <v>438800</v>
       </c>
       <c r="G2">
-        <v>428500</v>
+        <v>435000</v>
       </c>
       <c r="H2">
         <v>749</v>
       </c>
       <c r="I2">
-        <v>1483</v>
+        <v>1351</v>
       </c>
       <c r="J2">
-        <v>510.91</v>
+        <v>537.03</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -940,28 +940,28 @@
         <v>18</v>
       </c>
       <c r="C3">
-        <v>415616.3198671832</v>
+        <v>426447.5816266823</v>
       </c>
       <c r="D3">
-        <v>414881.6440951854</v>
+        <v>425909.9361497952</v>
       </c>
       <c r="E3">
-        <v>802.1979977753059</v>
+        <v>801.428320655354</v>
       </c>
       <c r="F3">
-        <v>429000</v>
+        <v>432000</v>
       </c>
       <c r="G3">
-        <v>430000</v>
+        <v>434000</v>
       </c>
       <c r="H3">
         <v>749</v>
       </c>
       <c r="I3">
-        <v>1807</v>
+        <v>1709</v>
       </c>
       <c r="J3">
-        <v>517.1799999999999</v>
+        <v>531.4400000000001</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -970,28 +970,28 @@
         <v>19</v>
       </c>
       <c r="C4">
-        <v>421724.0535077289</v>
+        <v>430891.138317757</v>
       </c>
       <c r="D4">
-        <v>420892.4309631391</v>
+        <v>430233.6279626168</v>
       </c>
       <c r="E4">
-        <v>799.8965929468021</v>
+        <v>798.5327102803739</v>
       </c>
       <c r="F4">
-        <v>434900</v>
+        <v>439000</v>
       </c>
       <c r="G4">
-        <v>435000</v>
+        <v>438588</v>
       </c>
       <c r="H4">
         <v>749</v>
       </c>
       <c r="I4">
-        <v>1682</v>
+        <v>1605</v>
       </c>
       <c r="J4">
-        <v>526.1799999999999</v>
+        <v>538.78</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -1000,28 +1000,28 @@
         <v>20</v>
       </c>
       <c r="C5">
-        <v>421431.3644408688</v>
+        <v>431979.1935483871</v>
       </c>
       <c r="D5">
-        <v>420847.1874497184</v>
+        <v>431607.3471986417</v>
       </c>
       <c r="E5">
-        <v>841.1401944894651</v>
+        <v>838.304753820034</v>
       </c>
       <c r="F5">
-        <v>435000</v>
+        <v>439700</v>
       </c>
       <c r="G5">
-        <v>438888</v>
+        <v>440000</v>
       </c>
       <c r="H5">
         <v>849</v>
       </c>
       <c r="I5">
-        <v>1243</v>
+        <v>1178</v>
       </c>
       <c r="J5">
-        <v>500.33</v>
+        <v>514.86</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -1449,28 +1449,28 @@
         <v>21</v>
       </c>
       <c r="C2">
-        <v>416098.9722572509</v>
+        <v>426104.2031662269</v>
       </c>
       <c r="D2">
-        <v>427529.5233417402</v>
+        <v>438234.8443403694</v>
       </c>
       <c r="E2">
-        <v>831.4216560509554</v>
+        <v>832.8733509234828</v>
       </c>
       <c r="F2">
-        <v>429000</v>
+        <v>429900</v>
       </c>
       <c r="G2">
-        <v>445000</v>
+        <v>448650</v>
       </c>
       <c r="H2">
         <v>849</v>
       </c>
       <c r="I2">
-        <v>793</v>
+        <v>758</v>
       </c>
       <c r="J2">
-        <v>514.22</v>
+        <v>526.17</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -1479,28 +1479,28 @@
         <v>22</v>
       </c>
       <c r="C3">
-        <v>431498.4012638231</v>
+        <v>440571.3618421053</v>
       </c>
       <c r="D3">
-        <v>430001.233807267</v>
+        <v>439270.6101973684</v>
       </c>
       <c r="E3">
-        <v>778.7939297124601</v>
+        <v>776.2220394736842</v>
       </c>
       <c r="F3">
         <v>449000</v>
       </c>
       <c r="G3">
-        <v>445000</v>
+        <v>448194</v>
       </c>
       <c r="H3">
         <v>749</v>
       </c>
       <c r="I3">
-        <v>633</v>
+        <v>608</v>
       </c>
       <c r="J3">
-        <v>552.14</v>
+        <v>565.91</v>
       </c>
     </row>
     <row r="4" spans="1:10">

</xml_diff>